<commit_message>
Made some graph related changes for manuscript
</commit_message>
<xml_diff>
--- a/LacTissue0222final_0412_recovered.xlsx
+++ b/LacTissue0222final_0412_recovered.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62896AB0-7F98-4E51-930A-6A512F7378B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCABBD9-F928-4B67-9B38-0531C76E75C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9CA065B6-2B6A-4D01-BE68-6D40353B42D4}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9CA065B6-2B6A-4D01-BE68-6D40353B42D4}"/>
   </bookViews>
   <sheets>
     <sheet name="TissueSlices" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
   <si>
     <t>Normal</t>
   </si>
@@ -5078,8 +5080,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49:H49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5087,9 +5089,10 @@
     <col min="1" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>2.0422959410288852E-2</v>
       </c>
@@ -5137,7 +5140,7 @@
         <v>3.5913379487449028E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2.0229842198082767E-2</v>
       </c>
@@ -5169,7 +5172,7 @@
         <v>0.17869625169151973</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2.113302655207866E-2</v>
       </c>
@@ -5200,8 +5203,24 @@
       <c r="J3" s="1">
         <v>0.25588656191366183</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S3">
+        <f>STDEV(G1,G8,G9,G11,G12,G13,G15,G16,G17)/COUNT(G1,G8,G9,G11,G12,G13,G15,G16,G17)</f>
+        <v>1.2776537307400389E-3</v>
+      </c>
+      <c r="T3">
+        <f>STDEV(H1,H8,H9,H11,H12,H13,H15,H16,H17)/COUNT(H1,H8,H9,H11,H12,H13,H15,H16,H17)</f>
+        <v>3.8042295738215373E-3</v>
+      </c>
+      <c r="U3">
+        <f>STDEV(I1,I8,I9,I11,I12,I13,I15,I16,I17)/COUNT(I1,I8,I9,I11,I12,I13,I15,I16,I17)</f>
+        <v>7.1910550920966975E-3</v>
+      </c>
+      <c r="V3">
+        <f>STDEV(J1,J8,J9,J11,J12,J13,J15,J16,J17)/COUNT(J1,J8,J9,J11,J12,J13,J15,J16,J17)</f>
+        <v>1.6758063198929116E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.9819112639040504E-2</v>
       </c>
@@ -5233,7 +5252,7 @@
         <v>0.14836296163036</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.9758981644190293E-2</v>
       </c>
@@ -5287,7 +5306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2.0494641965159224E-2</v>
       </c>
@@ -5339,7 +5358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2.0908399660504225E-2</v>
       </c>
@@ -5371,7 +5390,7 @@
         <v>0.27077335890718474</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2.1051891939320892E-2</v>
       </c>
@@ -5403,7 +5422,7 @@
         <v>0.13610334184766176</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2.0711806926558871E-2</v>
       </c>
@@ -5435,7 +5454,7 @@
         <v>0.15737580320906272</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2.059942882664062E-2</v>
       </c>
@@ -5475,7 +5494,7 @@
         <v>2.6573725181374009E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2.1026002836656291E-2</v>
       </c>
@@ -5513,7 +5532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2.0924689322908321E-2</v>
       </c>
@@ -5551,7 +5570,7 @@
         <v>37.631156082735345</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2.0000513463310804E-2</v>
       </c>
@@ -5591,7 +5610,7 @@
         <v>0.38251864512113587</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1.9678730436164599E-2</v>
       </c>
@@ -5631,7 +5650,7 @@
         <v>0.15815167446466222</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>1.9693344093520332E-2</v>
       </c>
@@ -5677,7 +5696,7 @@
         <v>0.38251864512113587</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2.074716373388065E-2</v>
       </c>
@@ -7018,11 +7037,197 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EC0785-D8ED-4308-8FFF-A093E18D5D27}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3.9161094915027964E-2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.1774127255788287E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1.9050934938391281E-3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.9461243767944972E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.3212211559969589</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.12182863024522686</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2.0150483733330233</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.24365726049045372</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="7">
+        <v>2.570581835636315</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA5D123-31A4-4532-9A5D-66B10C3D73C4}">
+  <dimension ref="B1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>0.11234249220155619</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2.4092865066039244E-14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>6.9498743102269062E-4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.9719610985541685E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>2.2924162416235652E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.2204460492503131E-14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>1.667705272509102E-2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2.7376898037565166E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>4.3166779801234297E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E606862-7454-458B-90DD-4839F350F2C8}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -7150,7 +7355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E250937D-150B-4FF5-B849-8A95789F3141}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C13"/>
@@ -7280,13 +7485,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0445B084-EDA1-4B5D-BAE6-2C7A1740166F}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7341,7 +7546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E9C258-26AC-4257-B8CD-A2925B80B800}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:U13"/>

</xml_diff>

<commit_message>
Getting repo ready to run tissue slices with benign sample added
</commit_message>
<xml_diff>
--- a/LacTissue0222final_0412_recovered.xlsx
+++ b/LacTissue0222final_0412_recovered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCABBD9-F928-4B67-9B38-0531C76E75C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5E5BDB-3A54-4292-804D-B5E1EE098305}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9CA065B6-2B6A-4D01-BE68-6D40353B42D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9CA065B6-2B6A-4D01-BE68-6D40353B42D4}"/>
   </bookViews>
   <sheets>
     <sheet name="TissueSlices" sheetId="1" r:id="rId1"/>
@@ -5080,7 +5080,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
@@ -7038,6 +7038,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EC0785-D8ED-4308-8FFF-A093E18D5D27}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7164,6 +7165,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA5D123-31A4-4532-9A5D-66B10C3D73C4}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>